<commit_message>
präsi für Hirschwang fertig machen
</commit_message>
<xml_diff>
--- a/data/prep_plots.xlsx
+++ b/data/prep_plots.xlsx
@@ -8,17 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wu-my.sharepoint.com/personal/clara_himmelbauer_wu_ac_at/Documents/Dokumente/hirschwang-hochrechnung/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="67" documentId="11_AD4DB114E441178AC67DF4B17E17FBBA683EDF24" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{44B5E245-B797-4E9A-B8BD-574D86402E37}"/>
+  <xr:revisionPtr revIDLastSave="96" documentId="11_AD4DB114E441178AC67DF4B17E17FBBA683EDF24" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0CCE9CBB-426D-4E4C-8C9A-7E7B906E5F87}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="urnenwahlergebnis_24" sheetId="1" r:id="rId1"/>
     <sheet name="lineare funktion" sheetId="2" r:id="rId2"/>
+    <sheet name="d'Hondt" sheetId="3" r:id="rId3"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId3"/>
-  </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">urnenwahlergebnis_24!$A$6:$D$6</definedName>
   </definedNames>
@@ -43,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
   <si>
     <t>wber</t>
   </si>
@@ -101,6 +99,15 @@
   <si>
     <t>Wald</t>
   </si>
+  <si>
+    <t>ohne sonstige</t>
+  </si>
+  <si>
+    <t>proportional</t>
+  </si>
+  <si>
+    <t>gewollt</t>
+  </si>
 </sst>
 </file>
 
@@ -146,10 +153,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Prozent" xfId="1" builtinId="5"/>
@@ -1562,6 +1570,403 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Palatino Linotype" panose="02040502050505030304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-AT" sz="1400" b="1"/>
+              <a:t>Mandatsverteilung im Nationalrat</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Palatino Linotype" panose="02040502050505030304" pitchFamily="18" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000004-94DC-4059-9101-4B3EBE8509EE}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-94DC-4059-9101-4B3EBE8509EE}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-94DC-4059-9101-4B3EBE8509EE}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-94DC-4059-9101-4B3EBE8509EE}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Palatino Linotype" panose="02040502050505030304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="de-DE"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'d''Hondt'!$B$8:$B$12</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>NEOS</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>GRÜNE</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FPÖ</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>SPÖ</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>ÖVP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'d''Hondt'!$H$8:$H$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>51</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-94DC-4059-9101-4B3EBE8509EE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="125"/>
+        <c:axId val="1601402895"/>
+        <c:axId val="1601403855"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1601402895"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Palatino Linotype" panose="02040502050505030304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1601403855"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1601403855"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1601402895"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:latin typeface="Palatino Linotype" panose="02040502050505030304" pitchFamily="18" charset="0"/>
+          <a:ea typeface="+mn-ea"/>
+          <a:cs typeface="+mn-cs"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1682,6 +2087,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
   <cs:axisTitle>
@@ -3200,6 +3645,511 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -3341,37 +4291,49 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="lineare funktion"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="2">
-          <cell r="B2">
-            <v>0.3</v>
-          </cell>
-          <cell r="C2">
-            <v>0.2</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="B3">
-            <v>0.5</v>
-          </cell>
-          <cell r="C3">
-            <v>0.45</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E5D80863-1A26-9576-016D-2943A306BD9D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3639,18 +4601,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -3658,7 +4620,7 @@
         <v>6346059</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -3666,7 +4628,7 @@
         <v>4753331</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>2</v>
       </c>
@@ -3674,7 +4636,7 @@
         <v>44954</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -3682,7 +4644,7 @@
         <v>4708377</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3697,7 +4659,7 @@
         <v>6.2673401046687643E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5</v>
       </c>
@@ -3712,7 +4674,7 @@
         <v>8.9619204239592534E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>4</v>
       </c>
@@ -3727,7 +4689,7 @@
         <v>8.030707821400028E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>3</v>
       </c>
@@ -3742,7 +4704,7 @@
         <v>0.2921333614534265</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2</v>
       </c>
@@ -3757,7 +4719,7 @@
         <v>0.2104941893990222</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
@@ -3787,13 +4749,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FA1C369-AD13-414D-8378-D156DC362884}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -3804,7 +4766,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -3815,7 +4777,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -3826,7 +4788,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -3837,7 +4799,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -3848,7 +4810,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -3863,4 +4825,214 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4C7D0B6-F7D2-4ECA-AB97-A3B9A685CF00}">
+  <dimension ref="A1:H12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>6346059</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>4753331</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>44954</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>4708377</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7">
+        <v>295090</v>
+      </c>
+      <c r="D7" s="1">
+        <f t="shared" ref="D7:D12" si="0">C7/$C$5</f>
+        <v>6.2673401046687643E-2</v>
+      </c>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8">
+        <v>421961</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" si="0"/>
+        <v>8.9619204239592534E-2</v>
+      </c>
+      <c r="F8" s="3">
+        <f>D8/SUM($D$8:$D$12)</f>
+        <v>9.5611502265771531E-2</v>
+      </c>
+      <c r="G8">
+        <f>F8*183</f>
+        <v>17.49690491463619</v>
+      </c>
+      <c r="H8">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>378116</v>
+      </c>
+      <c r="D9" s="1">
+        <f t="shared" si="0"/>
+        <v>8.030707821400028E-2</v>
+      </c>
+      <c r="F9" s="3">
+        <f t="shared" ref="F9:F12" si="1">D9/SUM($D$8:$D$12)</f>
+        <v>8.5676730291956993E-2</v>
+      </c>
+      <c r="G9">
+        <f t="shared" ref="G9:G12" si="2">F9*183</f>
+        <v>15.678841643428129</v>
+      </c>
+      <c r="H9">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10">
+        <v>1375474</v>
+      </c>
+      <c r="D10" s="1">
+        <f t="shared" si="0"/>
+        <v>0.2921333614534265</v>
+      </c>
+      <c r="F10" s="3">
+        <f t="shared" si="1"/>
+        <v>0.31166656507949742</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="2"/>
+        <v>57.034981409548024</v>
+      </c>
+      <c r="H10">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11">
+        <v>991086</v>
+      </c>
+      <c r="D11" s="1">
+        <f t="shared" si="0"/>
+        <v>0.2104941893990222</v>
+      </c>
+      <c r="F11" s="3">
+        <f t="shared" si="1"/>
+        <v>0.22456867183122242</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="2"/>
+        <v>41.096066945113705</v>
+      </c>
+      <c r="H11">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12">
+        <v>1246650</v>
+      </c>
+      <c r="D12" s="1">
+        <f t="shared" si="0"/>
+        <v>0.26477276564727081</v>
+      </c>
+      <c r="F12" s="3">
+        <f t="shared" si="1"/>
+        <v>0.2824765305315517</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="2"/>
+        <v>51.693205087273959</v>
+      </c>
+      <c r="H12">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>